<commit_message>
DataBase writeExcelFile method added
</commit_message>
<xml_diff>
--- a/src/main/DataBase/ClientDataBase.xlsx
+++ b/src/main/DataBase/ClientDataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray/Documents/git/ATM_Project/src/main/DataBase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D7AD2D-F32B-B04B-BCE1-924C67EEDFBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC70FEF-3B51-BC42-920B-120D3E00987F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -345,12 +345,12 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="14.5" style="2"/>
+    <col min="1" max="5" width="14.5" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Exit, Validation, Updated DataBase file
</commit_message>
<xml_diff>
--- a/src/main/DataBase/ClientDataBase.xlsx
+++ b/src/main/DataBase/ClientDataBase.xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray/Documents/git/ATM_Project/src/main/DataBase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC70FEF-3B51-BC42-920B-120D3E00987F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E289806F-5854-9146-84AE-BEEB6B552D76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Clients" sheetId="1" r:id="rId1"/>
+    <sheet name="Checkin" sheetId="3" r:id="rId2"/>
+    <sheet name="Saving" sheetId="2" r:id="rId3"/>
+    <sheet name="Money Market" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>Card Number</t>
   </si>
@@ -74,13 +88,79 @@
   </si>
   <si>
     <t>Spider Man</t>
+  </si>
+  <si>
+    <t>4444</t>
+  </si>
+  <si>
+    <t>5555</t>
+  </si>
+  <si>
+    <t>6666</t>
+  </si>
+  <si>
+    <t>7777</t>
+  </si>
+  <si>
+    <t>8888</t>
+  </si>
+  <si>
+    <t>9999</t>
+  </si>
+  <si>
+    <t>102920005</t>
+  </si>
+  <si>
+    <t>102920006</t>
+  </si>
+  <si>
+    <t>102920007</t>
+  </si>
+  <si>
+    <t>102920008</t>
+  </si>
+  <si>
+    <t>John Duck</t>
+  </si>
+  <si>
+    <t>Donald Powers</t>
+  </si>
+  <si>
+    <t>Austin Duck</t>
+  </si>
+  <si>
+    <t>John Powers</t>
+  </si>
+  <si>
+    <t>Ann Smith</t>
+  </si>
+  <si>
+    <t>102920001</t>
+  </si>
+  <si>
+    <t>102920009</t>
+  </si>
+  <si>
+    <t>102920010</t>
+  </si>
+  <si>
+    <t>104201#2839</t>
+  </si>
+  <si>
+    <t>104216#92</t>
+  </si>
+  <si>
+    <t>104219#0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -97,6 +177,10 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -119,11 +203,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,18 +427,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="106" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="5" width="14.5" style="2" collapsed="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -369,8 +457,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -383,11 +474,14 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1">
-        <v>102920001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -403,8 +497,11 @@
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -420,8 +517,11 @@
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -436,6 +536,426 @@
       </c>
       <c r="E5" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7642EA-03EF-994B-A1B4-2690F1276AED}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="10" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="str">
+        <f>Clients!E2</f>
+        <v>102920001</v>
+      </c>
+      <c r="B1" s="2" t="str">
+        <f>Clients!E3</f>
+        <v>102920002</v>
+      </c>
+      <c r="C1" s="2" t="str">
+        <f>Clients!E4</f>
+        <v>102920003</v>
+      </c>
+      <c r="D1" s="2" t="str">
+        <f>Clients!E5</f>
+        <v>102920004</v>
+      </c>
+      <c r="E1" s="2" t="str">
+        <f>Clients!E6</f>
+        <v>102920005</v>
+      </c>
+      <c r="F1" s="2" t="str">
+        <f>Clients!E7</f>
+        <v>102920006</v>
+      </c>
+      <c r="G1" s="2" t="str">
+        <f>Clients!E8</f>
+        <v>102920007</v>
+      </c>
+      <c r="H1" s="2" t="str">
+        <f>Clients!E9</f>
+        <v>102920008</v>
+      </c>
+      <c r="I1" s="2" t="str">
+        <f>Clients!E10</f>
+        <v>102920009</v>
+      </c>
+      <c r="J1" s="2" t="str">
+        <f>Clients!E11</f>
+        <v>102920010</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>104202</v>
+      </c>
+      <c r="C2">
+        <v>104203</v>
+      </c>
+      <c r="D2">
+        <v>104204</v>
+      </c>
+      <c r="E2">
+        <v>104205</v>
+      </c>
+      <c r="F2">
+        <v>104206</v>
+      </c>
+      <c r="G2">
+        <v>104207</v>
+      </c>
+      <c r="H2">
+        <v>104208</v>
+      </c>
+      <c r="I2">
+        <v>104209</v>
+      </c>
+      <c r="J2">
+        <v>104210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3">
+        <v>104215</v>
+      </c>
+      <c r="D3">
+        <v>104213</v>
+      </c>
+      <c r="G3">
+        <v>104214</v>
+      </c>
+      <c r="H3">
+        <v>104218</v>
+      </c>
+      <c r="I3">
+        <v>104212</v>
+      </c>
+      <c r="J3">
+        <v>104211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4">
+        <v>104217</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4819721-7DA6-2247-80DC-EBD6D162EA91}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="str">
+        <f>Clients!E2</f>
+        <v>102920001</v>
+      </c>
+      <c r="B1" s="2" t="str">
+        <f>Clients!E3</f>
+        <v>102920002</v>
+      </c>
+      <c r="C1" s="2" t="str">
+        <f>Clients!E4</f>
+        <v>102920003</v>
+      </c>
+      <c r="D1" s="2" t="str">
+        <f>Clients!E5</f>
+        <v>102920004</v>
+      </c>
+      <c r="E1" s="2" t="str">
+        <f>Clients!E6</f>
+        <v>102920005</v>
+      </c>
+      <c r="F1" s="2" t="str">
+        <f>Clients!E7</f>
+        <v>102920006</v>
+      </c>
+      <c r="G1" s="2" t="str">
+        <f>Clients!E8</f>
+        <v>102920007</v>
+      </c>
+      <c r="H1" s="2" t="str">
+        <f>Clients!E9</f>
+        <v>102920008</v>
+      </c>
+      <c r="I1" s="2" t="str">
+        <f>Clients!E10</f>
+        <v>102920009</v>
+      </c>
+      <c r="J1" s="2" t="str">
+        <f>Clients!E11</f>
+        <v>102920010</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>204201</v>
+      </c>
+      <c r="B2">
+        <v>204202</v>
+      </c>
+      <c r="C2">
+        <v>204203</v>
+      </c>
+      <c r="D2">
+        <v>204204</v>
+      </c>
+      <c r="E2">
+        <v>204205</v>
+      </c>
+      <c r="F2">
+        <v>204206</v>
+      </c>
+      <c r="G2">
+        <v>204207</v>
+      </c>
+      <c r="H2">
+        <v>204208</v>
+      </c>
+      <c r="I2">
+        <v>204209</v>
+      </c>
+      <c r="J2">
+        <v>204210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A670BC-E615-A949-BE17-7BE2778DAF06}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="str">
+        <f>Clients!E2</f>
+        <v>102920001</v>
+      </c>
+      <c r="B1" s="2" t="str">
+        <f>Clients!E3</f>
+        <v>102920002</v>
+      </c>
+      <c r="C1" s="2" t="str">
+        <f>Clients!E4</f>
+        <v>102920003</v>
+      </c>
+      <c r="D1" s="2" t="str">
+        <f>Clients!E5</f>
+        <v>102920004</v>
+      </c>
+      <c r="E1" s="2" t="str">
+        <f>Clients!E6</f>
+        <v>102920005</v>
+      </c>
+      <c r="F1" s="2" t="str">
+        <f>Clients!E7</f>
+        <v>102920006</v>
+      </c>
+      <c r="G1" s="2" t="str">
+        <f>Clients!E8</f>
+        <v>102920007</v>
+      </c>
+      <c r="H1" s="2" t="str">
+        <f>Clients!E9</f>
+        <v>102920008</v>
+      </c>
+      <c r="I1" s="2" t="str">
+        <f>Clients!E10</f>
+        <v>102920009</v>
+      </c>
+      <c r="J1" s="2" t="str">
+        <f>Clients!E11</f>
+        <v>102920010</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>304201</v>
+      </c>
+      <c r="B2">
+        <v>304202</v>
+      </c>
+      <c r="C2">
+        <v>304203</v>
+      </c>
+      <c r="D2">
+        <v>304204</v>
+      </c>
+      <c r="E2">
+        <v>304205</v>
+      </c>
+      <c r="F2">
+        <v>304206</v>
+      </c>
+      <c r="G2">
+        <v>304207</v>
+      </c>
+      <c r="H2">
+        <v>304208</v>
+      </c>
+      <c r="I2">
+        <v>304209</v>
+      </c>
+      <c r="J2">
+        <v>304210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DataBase writeExcelFile method fixed
</commit_message>
<xml_diff>
--- a/src/main/DataBase/ClientDataBase.xlsx
+++ b/src/main/DataBase/ClientDataBase.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray/Documents/git/ATM_Project/src/main/DataBase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E289806F-5854-9146-84AE-BEEB6B552D76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32033CD5-FF08-004F-805D-35EA228EA493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>Card Number</t>
   </si>
@@ -429,16 +429,16 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScale="106" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:N1048576"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="14.5" style="2" collapsed="1"/>
-    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" style="2" width="14.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.15">
@@ -486,7 +486,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -653,13 +653,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7642EA-03EF-994B-A1B4-2690F1276AED}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="10" width="18.6640625" customWidth="1"/>
+    <col min="1" max="10" customWidth="true" width="18.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
@@ -783,8 +783,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
latest update Ash Part
</commit_message>
<xml_diff>
--- a/src/main/DataBase/ClientDataBase.xlsx
+++ b/src/main/DataBase/ClientDataBase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray/Documents/git/ATM_Project/src/main/DataBase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32033CD5-FF08-004F-805D-35EA228EA493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5942D7C8-C774-1B49-9E64-290F02EBC8F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
   <si>
     <t>Card Number</t>
   </si>
@@ -151,6 +151,105 @@
   </si>
   <si>
     <t>104219#0</t>
+  </si>
+  <si>
+    <t>204203#3</t>
+  </si>
+  <si>
+    <t>204204#3</t>
+  </si>
+  <si>
+    <t>204205#3</t>
+  </si>
+  <si>
+    <t>204206#3</t>
+  </si>
+  <si>
+    <t>204207#3</t>
+  </si>
+  <si>
+    <t>204208#3</t>
+  </si>
+  <si>
+    <t>204209#3</t>
+  </si>
+  <si>
+    <t>204210#3</t>
+  </si>
+  <si>
+    <t>204212#1</t>
+  </si>
+  <si>
+    <t>204213#3</t>
+  </si>
+  <si>
+    <t>204214#3</t>
+  </si>
+  <si>
+    <t>2042013874#3</t>
+  </si>
+  <si>
+    <t>204211#23#2</t>
+  </si>
+  <si>
+    <t>204202#0#3</t>
+  </si>
+  <si>
+    <t>304201#543</t>
+  </si>
+  <si>
+    <t>304202#123456</t>
+  </si>
+  <si>
+    <t>304203#4354354</t>
+  </si>
+  <si>
+    <t>304204#40000</t>
+  </si>
+  <si>
+    <t>304205#2300</t>
+  </si>
+  <si>
+    <t>304206#0</t>
+  </si>
+  <si>
+    <t>304207#12</t>
+  </si>
+  <si>
+    <t>304208#45000</t>
+  </si>
+  <si>
+    <t>304209#2000000</t>
+  </si>
+  <si>
+    <t>304210#323232</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Acc#1</t>
+  </si>
+  <si>
+    <t>Acc#2</t>
+  </si>
+  <si>
+    <t>Acc#3</t>
+  </si>
+  <si>
+    <t>Acc#4</t>
+  </si>
+  <si>
+    <t>Acc#5</t>
+  </si>
+  <si>
+    <t>SavAcc</t>
+  </si>
+  <si>
+    <t>CheckAcc</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -430,15 +529,15 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" style="2" width="14.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.83203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="1" max="5" width="14.5" style="2" collapsed="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.15">
@@ -457,8 +556,12 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -477,8 +580,12 @@
       <c r="E2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -486,7 +593,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -497,8 +604,12 @@
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="F3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -517,8 +628,12 @@
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="F4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -537,8 +652,12 @@
       <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -557,6 +676,12 @@
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
@@ -574,6 +699,12 @@
       <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
@@ -591,6 +722,12 @@
       <c r="E8" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
@@ -608,6 +745,12 @@
       <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
@@ -625,6 +768,12 @@
       <c r="E10" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
@@ -641,6 +790,12 @@
       </c>
       <c r="E11" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -651,120 +806,142 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7642EA-03EF-994B-A1B4-2690F1276AED}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="10" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="2" max="11" width="15.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="str">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="2" t="str">
         <f>Clients!E2</f>
         <v>102920001</v>
       </c>
-      <c r="B1" s="2" t="str">
+      <c r="C1" s="2" t="str">
         <f>Clients!E3</f>
         <v>102920002</v>
       </c>
-      <c r="C1" s="2" t="str">
+      <c r="D1" s="2" t="str">
         <f>Clients!E4</f>
         <v>102920003</v>
       </c>
-      <c r="D1" s="2" t="str">
+      <c r="E1" s="2" t="str">
         <f>Clients!E5</f>
         <v>102920004</v>
       </c>
-      <c r="E1" s="2" t="str">
+      <c r="F1" s="2" t="str">
         <f>Clients!E6</f>
         <v>102920005</v>
       </c>
-      <c r="F1" s="2" t="str">
+      <c r="G1" s="2" t="str">
         <f>Clients!E7</f>
         <v>102920006</v>
       </c>
-      <c r="G1" s="2" t="str">
+      <c r="H1" s="2" t="str">
         <f>Clients!E8</f>
         <v>102920007</v>
       </c>
-      <c r="H1" s="2" t="str">
+      <c r="I1" s="2" t="str">
         <f>Clients!E9</f>
         <v>102920008</v>
       </c>
-      <c r="I1" s="2" t="str">
+      <c r="J1" s="2" t="str">
         <f>Clients!E10</f>
         <v>102920009</v>
       </c>
-      <c r="J1" s="2" t="str">
+      <c r="K1" s="2" t="str">
         <f>Clients!E11</f>
         <v>102920010</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
         <v>36</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>104202</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>104203</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>104204</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>104205</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>104206</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>104207</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>104208</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>104209</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>104210</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>104215</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>104213</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>104214</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>104218</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>104212</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>104211</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
         <v>38</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>104217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -775,187 +952,254 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4819721-7DA6-2247-80DC-EBD6D162EA91}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.83203125" collapsed="true"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="11" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="str">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="2" t="str">
         <f>Clients!E2</f>
         <v>102920001</v>
       </c>
-      <c r="B1" s="2" t="str">
+      <c r="C1" s="2" t="str">
         <f>Clients!E3</f>
         <v>102920002</v>
       </c>
-      <c r="C1" s="2" t="str">
+      <c r="D1" s="2" t="str">
         <f>Clients!E4</f>
         <v>102920003</v>
       </c>
-      <c r="D1" s="2" t="str">
+      <c r="E1" s="2" t="str">
         <f>Clients!E5</f>
         <v>102920004</v>
       </c>
-      <c r="E1" s="2" t="str">
+      <c r="F1" s="2" t="str">
         <f>Clients!E6</f>
         <v>102920005</v>
       </c>
-      <c r="F1" s="2" t="str">
+      <c r="G1" s="2" t="str">
         <f>Clients!E7</f>
         <v>102920006</v>
       </c>
-      <c r="G1" s="2" t="str">
+      <c r="H1" s="2" t="str">
         <f>Clients!E8</f>
         <v>102920007</v>
       </c>
-      <c r="H1" s="2" t="str">
+      <c r="I1" s="2" t="str">
         <f>Clients!E9</f>
         <v>102920008</v>
       </c>
-      <c r="I1" s="2" t="str">
+      <c r="J1" s="2" t="str">
         <f>Clients!E10</f>
         <v>102920009</v>
       </c>
-      <c r="J1" s="2" t="str">
+      <c r="K1" s="2" t="str">
         <f>Clients!E11</f>
         <v>102920010</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A2">
-        <v>204201</v>
-      </c>
-      <c r="B2">
-        <v>204202</v>
-      </c>
-      <c r="C2">
-        <v>204203</v>
-      </c>
-      <c r="D2">
-        <v>204204</v>
-      </c>
-      <c r="E2">
-        <v>204205</v>
-      </c>
-      <c r="F2">
-        <v>204206</v>
-      </c>
-      <c r="G2">
-        <v>204207</v>
-      </c>
-      <c r="H2">
-        <v>204208</v>
-      </c>
-      <c r="I2">
-        <v>204209</v>
-      </c>
-      <c r="J2">
-        <v>204210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="4"/>
-      <c r="D4" s="4"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A670BC-E615-A949-BE17-7BE2778DAF06}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="11" width="15.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="str">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="2" t="str">
         <f>Clients!E2</f>
         <v>102920001</v>
       </c>
-      <c r="B1" s="2" t="str">
+      <c r="C1" s="2" t="str">
         <f>Clients!E3</f>
         <v>102920002</v>
       </c>
-      <c r="C1" s="2" t="str">
+      <c r="D1" s="2" t="str">
         <f>Clients!E4</f>
         <v>102920003</v>
       </c>
-      <c r="D1" s="2" t="str">
+      <c r="E1" s="2" t="str">
         <f>Clients!E5</f>
         <v>102920004</v>
       </c>
-      <c r="E1" s="2" t="str">
+      <c r="F1" s="2" t="str">
         <f>Clients!E6</f>
         <v>102920005</v>
       </c>
-      <c r="F1" s="2" t="str">
+      <c r="G1" s="2" t="str">
         <f>Clients!E7</f>
         <v>102920006</v>
       </c>
-      <c r="G1" s="2" t="str">
+      <c r="H1" s="2" t="str">
         <f>Clients!E8</f>
         <v>102920007</v>
       </c>
-      <c r="H1" s="2" t="str">
+      <c r="I1" s="2" t="str">
         <f>Clients!E9</f>
         <v>102920008</v>
       </c>
-      <c r="I1" s="2" t="str">
+      <c r="J1" s="2" t="str">
         <f>Clients!E10</f>
         <v>102920009</v>
       </c>
-      <c r="J1" s="2" t="str">
+      <c r="K1" s="2" t="str">
         <f>Clients!E11</f>
         <v>102920010</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A2">
-        <v>304201</v>
-      </c>
-      <c r="B2">
-        <v>304202</v>
-      </c>
-      <c r="C2">
-        <v>304203</v>
-      </c>
-      <c r="D2">
-        <v>304204</v>
-      </c>
-      <c r="E2">
-        <v>304205</v>
-      </c>
-      <c r="F2">
-        <v>304206</v>
-      </c>
-      <c r="G2">
-        <v>304207</v>
-      </c>
-      <c r="H2">
-        <v>304208</v>
-      </c>
-      <c r="I2">
-        <v>304209</v>
-      </c>
-      <c r="J2">
-        <v>304210</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>